<commit_message>
Filled empty cells in size column
</commit_message>
<xml_diff>
--- a/Multi-taxa_data/MollEchino/Mol_raw/Mol_div_HI.xlsx
+++ b/Multi-taxa_data/MollEchino/Mol_raw/Mol_div_HI.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\claud\Documents\COMUNE\STUDIO.LAVORO\IMBRSea\Thesis\StatAnalysis\Multi-taxa_data\MollEchino\Mol_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{222EE600-A436-45CC-8A71-FB5DF857EBAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF1B10C8-BA3F-4F5E-AF69-F4656BA03338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1288" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1294" uniqueCount="138">
   <si>
     <t>transect</t>
   </si>
@@ -748,8 +748,8 @@
   </sheetPr>
   <dimension ref="A1:M1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A153" workbookViewId="0">
+      <selection activeCell="K135" sqref="K135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1381,6 +1381,9 @@
       </c>
       <c r="G22" s="3"/>
       <c r="J22" s="3"/>
+      <c r="K22" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
@@ -1711,6 +1714,9 @@
       </c>
       <c r="G34" s="3"/>
       <c r="J34" s="3"/>
+      <c r="K34" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="35" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
@@ -2591,7 +2597,9 @@
         <v>15</v>
       </c>
       <c r="G65" s="3"/>
-      <c r="K65" s="3"/>
+      <c r="K65" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="66" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
@@ -2639,7 +2647,9 @@
         <v>15</v>
       </c>
       <c r="G67" s="3"/>
-      <c r="K67" s="3"/>
+      <c r="K67" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="68" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
@@ -4533,6 +4543,9 @@
       <c r="J135" s="2" t="s">
         <v>129</v>
       </c>
+      <c r="K135" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="136" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
@@ -5232,6 +5245,9 @@
         <v>56</v>
       </c>
       <c r="G160" s="3"/>
+      <c r="K160" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="161" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">

</xml_diff>